<commit_message>
Cambios en N3 y N6
</commit_message>
<xml_diff>
--- a/Calificaciones 2025-2026/N3_ENS_C.xlsx
+++ b/Calificaciones 2025-2026/N3_ENS_C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GSE2GA\Documents\Personal\Tere Guerra\Meraki\Calificaciones 2025-2026\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\activ\Documents\Meraki\Calificaciones 2025-2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5492DE-B419-43AA-AA86-B6194DF8518B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16DF42B-1CA3-4759-95BF-BBB0640B5D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B2EF7373-A7E6-423B-9BCC-817B77FBEC7D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B2EF7373-A7E6-423B-9BCC-817B77FBEC7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Calificaciones" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
   <si>
     <t>No.</t>
   </si>
@@ -142,9 +142,6 @@
     <t>C1</t>
   </si>
   <si>
-    <t>Martes 9/9/2025                  La Polinización</t>
-  </si>
-  <si>
     <t>Miércoles 10/9/2025 Explorando mi Comunidad</t>
   </si>
   <si>
@@ -190,13 +187,40 @@
     <t>Jueves 23/10/2025         Tengo necesidades y derechos</t>
   </si>
   <si>
-    <t>Martes 4/11/2025               Mis necesidades y derechos</t>
-  </si>
-  <si>
     <t>Miércoles 5/11/2025         Mis necesidades y derechos</t>
   </si>
   <si>
     <t>Ética, naturaleza y sociedades Libro 1</t>
+  </si>
+  <si>
+    <t>Martes 9/9/2025                      La Polinización</t>
+  </si>
+  <si>
+    <t>Martes 4/11/2025                       Mis necesidades y derechos</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lunes 10/11/2025</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Evaluación</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -206,7 +230,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,8 +272,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,6 +321,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -357,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -382,106 +420,99 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,7 +536,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -823,11 +854,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AECF9521-3E5C-4485-A0EE-99CC705EEB69}">
   <dimension ref="B2:M16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -841,22 +872,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
@@ -952,10 +983,10 @@
       <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <v>6</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="9">
         <v>8</v>
       </c>
       <c r="G6" s="9">
@@ -969,7 +1000,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="9">
-        <f>'Libro 1'!AE7*0.5</f>
+        <f>'Libro 1'!AF7*0.5</f>
         <v>0</v>
       </c>
       <c r="K6" s="9">
@@ -991,10 +1022,10 @@
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="9">
         <v>9</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="9">
         <v>7</v>
       </c>
       <c r="G7" s="9">
@@ -1008,7 +1039,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="9">
-        <f>'Libro 1'!AE8*0.5</f>
+        <f>'Libro 1'!AF8*0.5</f>
         <v>0</v>
       </c>
       <c r="K7" s="9">
@@ -1030,10 +1061,10 @@
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="9">
         <v>4</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="9">
         <v>2</v>
       </c>
       <c r="G8" s="9">
@@ -1047,7 +1078,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="9">
-        <f>'Libro 1'!AE9*0.5</f>
+        <f>'Libro 1'!AF9*0.5</f>
         <v>0</v>
       </c>
       <c r="K8" s="9">
@@ -1069,10 +1100,10 @@
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="9">
         <v>9</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="9">
         <v>3</v>
       </c>
       <c r="G9" s="9">
@@ -1086,7 +1117,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="9">
-        <f>'Libro 1'!AE10*0.5</f>
+        <f>'Libro 1'!AF10*0.5</f>
         <v>3.38</v>
       </c>
       <c r="K9" s="9">
@@ -1108,10 +1139,10 @@
       <c r="D10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="9">
         <v>9</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="9">
         <v>7</v>
       </c>
       <c r="G10" s="9">
@@ -1125,15 +1156,15 @@
         <v>0</v>
       </c>
       <c r="J10" s="9">
-        <f>'Libro 1'!AE11*0.5</f>
-        <v>0</v>
+        <f>'Libro 1'!AF11*0.5</f>
+        <v>3.4</v>
       </c>
       <c r="K10" s="9">
         <v>0</v>
       </c>
       <c r="L10" s="11">
         <f t="shared" si="0"/>
-        <v>1.44</v>
+        <v>2.12</v>
       </c>
       <c r="M10" s="1"/>
     </row>
@@ -1147,10 +1178,10 @@
       <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="12">
-        <v>10</v>
-      </c>
-      <c r="F11" s="12">
+      <c r="E11" s="9">
+        <v>10</v>
+      </c>
+      <c r="F11" s="9">
         <v>9</v>
       </c>
       <c r="G11" s="9">
@@ -1164,7 +1195,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="9">
-        <f>'Libro 1'!AE12*0.5</f>
+        <f>'Libro 1'!AF12*0.5</f>
         <v>0</v>
       </c>
       <c r="K11" s="9">
@@ -1186,10 +1217,10 @@
       <c r="D12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="9">
         <v>5</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="9">
         <v>9</v>
       </c>
       <c r="G12" s="9">
@@ -1203,7 +1234,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="9">
-        <f>'Libro 1'!AE13*0.5</f>
+        <f>'Libro 1'!AF13*0.5</f>
         <v>0</v>
       </c>
       <c r="K12" s="9">
@@ -1225,10 +1256,10 @@
       <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="9">
         <v>4</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="9">
         <v>6</v>
       </c>
       <c r="G13" s="9">
@@ -1242,15 +1273,15 @@
         <v>0</v>
       </c>
       <c r="J13" s="9">
-        <f>'Libro 1'!AE14*0.5</f>
-        <v>0</v>
+        <f>'Libro 1'!AF14*0.5</f>
+        <v>3.8</v>
       </c>
       <c r="K13" s="9">
         <v>0</v>
       </c>
       <c r="L13" s="11">
         <f t="shared" si="0"/>
-        <v>0.9</v>
+        <v>1.6600000000000001</v>
       </c>
       <c r="M13" s="1"/>
     </row>
@@ -1264,10 +1295,10 @@
       <c r="D14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="9">
         <v>9</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="9">
         <v>9</v>
       </c>
       <c r="G14" s="9">
@@ -1281,15 +1312,15 @@
         <v>0</v>
       </c>
       <c r="J14" s="9">
-        <f>'Libro 1'!AE15*0.5</f>
-        <v>0</v>
+        <f>'Libro 1'!AF15*0.5</f>
+        <v>3.2</v>
       </c>
       <c r="K14" s="9">
         <v>0</v>
       </c>
       <c r="L14" s="11">
         <f t="shared" si="0"/>
-        <v>1.6199999999999999</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="M14" s="1"/>
     </row>
@@ -1303,10 +1334,10 @@
       <c r="D15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="9">
         <v>6</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="9">
         <v>7</v>
       </c>
       <c r="G15" s="9">
@@ -1320,7 +1351,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="9">
-        <f>'Libro 1'!AE16*0.5</f>
+        <f>'Libro 1'!AF16*0.5</f>
         <v>0</v>
       </c>
       <c r="K15" s="9">
@@ -1333,44 +1364,44 @@
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="14">
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="13">
         <f>AVERAGE(E6:E15)</f>
         <v>7.1</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="13">
         <f>AVERAGE(F6:F15)</f>
         <v>6.7</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="13">
         <f>AVERAGE(G7:G15)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="13">
         <f t="shared" ref="H16:L16" si="1">AVERAGE(H6:H15)</f>
         <v>0</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="13">
         <f t="shared" si="1"/>
-        <v>0.33799999999999997</v>
-      </c>
-      <c r="K16" s="14">
+        <v>1.3779999999999997</v>
+      </c>
+      <c r="K16" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="13">
         <f t="shared" si="1"/>
-        <v>1.3096000000000001</v>
-      </c>
-      <c r="M16" s="13"/>
+        <v>1.5176000000000001</v>
+      </c>
+      <c r="M16" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1385,283 +1416,290 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BFD2BAD-81F2-42F0-8CA8-62AE2AD1DE5C}">
-  <dimension ref="B2:AE16"/>
+  <dimension ref="B2:AF16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH4" sqref="AH4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AD20" sqref="AD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.5703125" customWidth="1"/>
     <col min="13" max="13" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="20" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="4.5703125" customWidth="1"/>
     <col min="22" max="22" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="7.7109375" customWidth="1"/>
     <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="27" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B2" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-    </row>
-    <row r="3" spans="2:31" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+    </row>
+    <row r="3" spans="2:32" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="31"/>
-      <c r="K3" s="29" t="s">
+      <c r="J3" s="38"/>
+      <c r="K3" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="38"/>
+      <c r="M3" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="31"/>
-      <c r="M3" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="32" t="s">
+      <c r="P3" s="39"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" s="38"/>
+      <c r="T3" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="29" t="s">
+      <c r="U3" s="38"/>
+      <c r="V3" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="X3" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="S3" s="31"/>
-      <c r="T3" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="U3" s="31"/>
-      <c r="V3" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="W3" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="X3" s="41" t="s">
+      <c r="Y3" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="Y3" s="29" t="s">
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="Z3" s="31"/>
-      <c r="AA3" s="32" t="s">
+      <c r="AB3" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="AB3" s="32" t="s">
+      <c r="AC3" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="AC3" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD3" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE3" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE3" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF3" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="26" t="s">
+      <c r="D4" s="20"/>
+      <c r="E4" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="26" t="s">
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="27"/>
-      <c r="K4" s="26" t="s">
+      <c r="J4" s="40"/>
+      <c r="K4" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="27"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="34" t="s">
+      <c r="L4" s="40"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" s="36"/>
+      <c r="T4" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" s="36"/>
+      <c r="V4" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="W4" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="X4" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="26" t="s">
+      <c r="Y4" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="S4" s="28"/>
-      <c r="T4" s="26" t="s">
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="U4" s="28"/>
-      <c r="V4" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="W4" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="X4" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y4" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z4" s="28"/>
-      <c r="AA4" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB4" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC4" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD4" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE4" s="8"/>
-    </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AB4" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC4" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD4" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE4" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF4" s="8"/>
+    </row>
+    <row r="5" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="18">
         <v>50</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="18">
         <v>51</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="18">
         <v>52</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="18">
         <v>53</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="18">
         <v>54</v>
       </c>
-      <c r="J5" s="21">
+      <c r="J5" s="18">
         <v>55</v>
       </c>
-      <c r="K5" s="21">
+      <c r="K5" s="18">
         <v>56</v>
       </c>
-      <c r="L5" s="21">
+      <c r="L5" s="18">
         <v>57</v>
       </c>
-      <c r="M5" s="22"/>
-      <c r="N5" s="21">
+      <c r="M5" s="19"/>
+      <c r="N5" s="18">
         <v>28</v>
       </c>
-      <c r="O5" s="21">
+      <c r="O5" s="18">
         <v>29</v>
       </c>
-      <c r="P5" s="21">
+      <c r="P5" s="18">
         <v>30</v>
       </c>
-      <c r="Q5" s="21">
+      <c r="Q5" s="18">
         <v>31</v>
       </c>
-      <c r="R5" s="21">
+      <c r="R5" s="18">
         <v>32</v>
       </c>
-      <c r="S5" s="21">
+      <c r="S5" s="18">
         <v>33</v>
       </c>
-      <c r="T5" s="21">
+      <c r="T5" s="18">
         <v>34</v>
       </c>
-      <c r="U5" s="21">
+      <c r="U5" s="18">
         <v>35</v>
       </c>
-      <c r="V5" s="21">
+      <c r="V5" s="18">
         <v>42</v>
       </c>
-      <c r="W5" s="21">
+      <c r="W5" s="18">
         <v>20</v>
       </c>
-      <c r="X5" s="39">
+      <c r="X5" s="29">
         <v>21</v>
       </c>
-      <c r="Y5" s="21">
+      <c r="Y5" s="18">
         <v>22</v>
       </c>
-      <c r="Z5" s="21">
+      <c r="Z5" s="18">
         <v>23</v>
       </c>
-      <c r="AA5" s="21">
+      <c r="AA5" s="18">
         <v>24</v>
       </c>
-      <c r="AB5" s="43">
+      <c r="AB5" s="18">
         <v>25</v>
       </c>
-      <c r="AC5" s="43">
+      <c r="AC5" s="18">
         <v>26</v>
       </c>
-      <c r="AD5" s="21">
+      <c r="AD5" s="18">
         <v>27</v>
       </c>
-      <c r="AE5" s="23"/>
-    </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AE5" s="18">
+        <v>40</v>
+      </c>
+      <c r="AF5" s="20"/>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1671,35 +1709,36 @@
       <c r="D6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="38"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="21"/>
-      <c r="AA6" s="21"/>
-      <c r="AB6" s="43"/>
-      <c r="AC6" s="21"/>
-      <c r="AD6" s="21"/>
-      <c r="AE6" s="20"/>
-    </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="28"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="18"/>
+      <c r="AB6" s="18"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="18"/>
+      <c r="AE6" s="18"/>
+      <c r="AF6" s="17"/>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>1</v>
       </c>
@@ -1709,88 +1748,89 @@
       <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="18">
-        <v>0</v>
-      </c>
-      <c r="F7" s="18">
-        <v>0</v>
-      </c>
-      <c r="G7" s="18">
-        <v>0</v>
-      </c>
-      <c r="H7" s="18">
-        <v>0</v>
-      </c>
-      <c r="I7" s="18">
-        <v>0</v>
-      </c>
-      <c r="J7" s="18">
-        <v>0</v>
-      </c>
-      <c r="K7" s="18">
-        <v>0</v>
-      </c>
-      <c r="L7" s="18">
-        <v>0</v>
-      </c>
-      <c r="M7" s="19"/>
-      <c r="N7" s="18">
-        <v>0</v>
-      </c>
-      <c r="O7" s="18">
-        <v>0</v>
-      </c>
-      <c r="P7" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="18">
-        <v>0</v>
-      </c>
-      <c r="R7" s="18">
-        <v>0</v>
-      </c>
-      <c r="S7" s="18">
-        <v>0</v>
-      </c>
-      <c r="T7" s="18">
-        <v>0</v>
-      </c>
-      <c r="U7" s="18">
-        <v>0</v>
-      </c>
-      <c r="V7" s="18">
-        <v>0</v>
-      </c>
-      <c r="W7" s="18">
-        <v>0</v>
-      </c>
-      <c r="X7" s="18">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="17">
-        <f>AVERAGE(E7:AD7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="E7" s="15">
+        <v>0</v>
+      </c>
+      <c r="F7" s="15">
+        <v>0</v>
+      </c>
+      <c r="G7" s="15">
+        <v>0</v>
+      </c>
+      <c r="H7" s="15">
+        <v>0</v>
+      </c>
+      <c r="I7" s="15">
+        <v>0</v>
+      </c>
+      <c r="J7" s="15">
+        <v>0</v>
+      </c>
+      <c r="K7" s="15">
+        <v>0</v>
+      </c>
+      <c r="L7" s="15">
+        <v>0</v>
+      </c>
+      <c r="M7" s="16"/>
+      <c r="N7" s="15">
+        <v>0</v>
+      </c>
+      <c r="O7" s="15">
+        <v>0</v>
+      </c>
+      <c r="P7" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="15">
+        <v>0</v>
+      </c>
+      <c r="R7" s="15">
+        <v>0</v>
+      </c>
+      <c r="S7" s="15">
+        <v>0</v>
+      </c>
+      <c r="T7" s="15">
+        <v>0</v>
+      </c>
+      <c r="U7" s="15">
+        <v>0</v>
+      </c>
+      <c r="V7" s="15">
+        <v>0</v>
+      </c>
+      <c r="W7" s="15">
+        <v>0</v>
+      </c>
+      <c r="X7" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="15"/>
+      <c r="AF7" s="14">
+        <f t="shared" ref="AF7:AF16" si="0">AVERAGE(E7:AD7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>2</v>
       </c>
@@ -1800,88 +1840,89 @@
       <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="18">
-        <v>0</v>
-      </c>
-      <c r="F8" s="18">
-        <v>0</v>
-      </c>
-      <c r="G8" s="18">
-        <v>0</v>
-      </c>
-      <c r="H8" s="18">
-        <v>0</v>
-      </c>
-      <c r="I8" s="18">
-        <v>0</v>
-      </c>
-      <c r="J8" s="18">
-        <v>0</v>
-      </c>
-      <c r="K8" s="18">
-        <v>0</v>
-      </c>
-      <c r="L8" s="18">
-        <v>0</v>
-      </c>
-      <c r="M8" s="19"/>
-      <c r="N8" s="18">
-        <v>0</v>
-      </c>
-      <c r="O8" s="18">
-        <v>0</v>
-      </c>
-      <c r="P8" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="18">
-        <v>0</v>
-      </c>
-      <c r="R8" s="18">
-        <v>0</v>
-      </c>
-      <c r="S8" s="18">
-        <v>0</v>
-      </c>
-      <c r="T8" s="18">
-        <v>0</v>
-      </c>
-      <c r="U8" s="18">
-        <v>0</v>
-      </c>
-      <c r="V8" s="18">
-        <v>0</v>
-      </c>
-      <c r="W8" s="18">
-        <v>0</v>
-      </c>
-      <c r="X8" s="18">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="17">
-        <f>AVERAGE(E8:AD8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="E8" s="41">
+        <v>0</v>
+      </c>
+      <c r="F8" s="41">
+        <v>0</v>
+      </c>
+      <c r="G8" s="41">
+        <v>0</v>
+      </c>
+      <c r="H8" s="41">
+        <v>0</v>
+      </c>
+      <c r="I8" s="41">
+        <v>0</v>
+      </c>
+      <c r="J8" s="41">
+        <v>0</v>
+      </c>
+      <c r="K8" s="41">
+        <v>0</v>
+      </c>
+      <c r="L8" s="41">
+        <v>0</v>
+      </c>
+      <c r="M8" s="16"/>
+      <c r="N8" s="41">
+        <v>0</v>
+      </c>
+      <c r="O8" s="41">
+        <v>0</v>
+      </c>
+      <c r="P8" s="41">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="41">
+        <v>0</v>
+      </c>
+      <c r="R8" s="41">
+        <v>0</v>
+      </c>
+      <c r="S8" s="41">
+        <v>0</v>
+      </c>
+      <c r="T8" s="41">
+        <v>0</v>
+      </c>
+      <c r="U8" s="41">
+        <v>0</v>
+      </c>
+      <c r="V8" s="41">
+        <v>0</v>
+      </c>
+      <c r="W8" s="41">
+        <v>0</v>
+      </c>
+      <c r="X8" s="41">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="41">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="41">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="41">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="41">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="41">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="41"/>
+      <c r="AF8" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>3</v>
       </c>
@@ -1891,179 +1932,181 @@
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="18">
-        <v>0</v>
-      </c>
-      <c r="F9" s="18">
-        <v>0</v>
-      </c>
-      <c r="G9" s="18">
-        <v>0</v>
-      </c>
-      <c r="H9" s="18">
-        <v>0</v>
-      </c>
-      <c r="I9" s="18">
-        <v>0</v>
-      </c>
-      <c r="J9" s="18">
-        <v>0</v>
-      </c>
-      <c r="K9" s="18">
-        <v>0</v>
-      </c>
-      <c r="L9" s="18">
-        <v>0</v>
-      </c>
-      <c r="M9" s="19"/>
-      <c r="N9" s="18">
-        <v>0</v>
-      </c>
-      <c r="O9" s="18">
-        <v>0</v>
-      </c>
-      <c r="P9" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="18">
-        <v>0</v>
-      </c>
-      <c r="R9" s="18">
-        <v>0</v>
-      </c>
-      <c r="S9" s="18">
-        <v>0</v>
-      </c>
-      <c r="T9" s="18">
-        <v>0</v>
-      </c>
-      <c r="U9" s="18">
-        <v>0</v>
-      </c>
-      <c r="V9" s="18">
-        <v>0</v>
-      </c>
-      <c r="W9" s="18">
-        <v>0</v>
-      </c>
-      <c r="X9" s="18">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="17">
-        <f>AVERAGE(E9:AD9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B10" s="44">
+      <c r="E9" s="15">
+        <v>0</v>
+      </c>
+      <c r="F9" s="15">
+        <v>0</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0</v>
+      </c>
+      <c r="H9" s="15">
+        <v>0</v>
+      </c>
+      <c r="I9" s="15">
+        <v>0</v>
+      </c>
+      <c r="J9" s="15">
+        <v>0</v>
+      </c>
+      <c r="K9" s="15">
+        <v>0</v>
+      </c>
+      <c r="L9" s="15">
+        <v>0</v>
+      </c>
+      <c r="M9" s="16"/>
+      <c r="N9" s="15">
+        <v>0</v>
+      </c>
+      <c r="O9" s="15">
+        <v>0</v>
+      </c>
+      <c r="P9" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="15">
+        <v>0</v>
+      </c>
+      <c r="R9" s="15">
+        <v>0</v>
+      </c>
+      <c r="S9" s="15">
+        <v>0</v>
+      </c>
+      <c r="T9" s="15">
+        <v>0</v>
+      </c>
+      <c r="U9" s="15">
+        <v>0</v>
+      </c>
+      <c r="V9" s="15">
+        <v>0</v>
+      </c>
+      <c r="W9" s="15">
+        <v>0</v>
+      </c>
+      <c r="X9" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="15"/>
+      <c r="AF9" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
         <v>4</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="5">
         <v>986</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="37">
-        <v>0</v>
-      </c>
-      <c r="F10" s="37">
-        <v>0</v>
-      </c>
-      <c r="G10" s="37">
-        <v>0</v>
-      </c>
-      <c r="H10" s="37">
-        <v>0</v>
-      </c>
-      <c r="I10" s="36">
-        <v>10</v>
-      </c>
-      <c r="J10" s="33">
-        <v>10</v>
-      </c>
-      <c r="K10" s="36">
-        <v>10</v>
-      </c>
-      <c r="L10" s="33">
+      <c r="E10" s="27">
+        <v>0</v>
+      </c>
+      <c r="F10" s="27">
+        <v>0</v>
+      </c>
+      <c r="G10" s="27">
+        <v>0</v>
+      </c>
+      <c r="H10" s="27">
+        <v>0</v>
+      </c>
+      <c r="I10" s="15">
+        <v>10</v>
+      </c>
+      <c r="J10" s="25">
+        <v>10</v>
+      </c>
+      <c r="K10" s="15">
+        <v>10</v>
+      </c>
+      <c r="L10" s="25">
         <v>7</v>
       </c>
-      <c r="M10" s="19"/>
-      <c r="N10" s="36">
-        <v>10</v>
-      </c>
-      <c r="O10" s="36">
-        <v>10</v>
-      </c>
-      <c r="P10" s="36">
+      <c r="M10" s="16"/>
+      <c r="N10" s="15">
+        <v>10</v>
+      </c>
+      <c r="O10" s="15">
+        <v>10</v>
+      </c>
+      <c r="P10" s="15">
         <v>9</v>
       </c>
-      <c r="Q10" s="36">
+      <c r="Q10" s="15">
         <v>8</v>
       </c>
-      <c r="R10" s="36">
-        <v>10</v>
-      </c>
-      <c r="S10" s="36">
-        <v>10</v>
-      </c>
-      <c r="T10" s="35">
-        <v>0</v>
-      </c>
-      <c r="U10" s="37">
-        <v>0</v>
-      </c>
-      <c r="V10" s="36">
+      <c r="R10" s="15">
+        <v>10</v>
+      </c>
+      <c r="S10" s="15">
+        <v>10</v>
+      </c>
+      <c r="T10" s="26">
+        <v>0</v>
+      </c>
+      <c r="U10" s="27">
+        <v>0</v>
+      </c>
+      <c r="V10" s="15">
         <v>7</v>
       </c>
-      <c r="W10" s="36">
-        <v>10</v>
-      </c>
-      <c r="X10" s="42">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="36">
-        <v>10</v>
-      </c>
-      <c r="Z10" s="36">
-        <v>10</v>
-      </c>
-      <c r="AA10" s="33">
+      <c r="W10" s="15">
+        <v>10</v>
+      </c>
+      <c r="X10" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="15">
+        <v>10</v>
+      </c>
+      <c r="Z10" s="15">
+        <v>10</v>
+      </c>
+      <c r="AA10" s="25">
         <v>8</v>
       </c>
-      <c r="AB10" s="36">
-        <v>10</v>
-      </c>
-      <c r="AC10" s="36">
-        <v>10</v>
-      </c>
-      <c r="AD10" s="36">
-        <v>10</v>
-      </c>
-      <c r="AE10" s="17">
-        <f>AVERAGE(E10:AD10)</f>
+      <c r="AB10" s="15">
+        <v>10</v>
+      </c>
+      <c r="AC10" s="15">
+        <v>10</v>
+      </c>
+      <c r="AD10" s="15">
+        <v>10</v>
+      </c>
+      <c r="AE10" s="15"/>
+      <c r="AF10" s="14">
+        <f t="shared" si="0"/>
         <v>6.76</v>
       </c>
     </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>5</v>
       </c>
@@ -2073,88 +2116,89 @@
       <c r="D11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="18">
-        <v>0</v>
-      </c>
-      <c r="F11" s="18">
-        <v>0</v>
-      </c>
-      <c r="G11" s="18">
-        <v>0</v>
-      </c>
-      <c r="H11" s="18">
-        <v>0</v>
-      </c>
-      <c r="I11" s="18">
-        <v>0</v>
-      </c>
-      <c r="J11" s="18">
-        <v>0</v>
-      </c>
-      <c r="K11" s="18">
-        <v>0</v>
-      </c>
-      <c r="L11" s="18">
-        <v>0</v>
-      </c>
-      <c r="M11" s="19"/>
-      <c r="N11" s="18">
-        <v>0</v>
-      </c>
-      <c r="O11" s="18">
-        <v>0</v>
-      </c>
-      <c r="P11" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="18">
-        <v>0</v>
-      </c>
-      <c r="R11" s="18">
-        <v>0</v>
-      </c>
-      <c r="S11" s="18">
-        <v>0</v>
-      </c>
-      <c r="T11" s="18">
-        <v>0</v>
-      </c>
-      <c r="U11" s="18">
-        <v>0</v>
-      </c>
-      <c r="V11" s="18">
-        <v>0</v>
-      </c>
-      <c r="W11" s="18">
-        <v>0</v>
-      </c>
-      <c r="X11" s="18">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="17">
-        <f>AVERAGE(E11:AD11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="E11" s="27">
+        <v>0</v>
+      </c>
+      <c r="F11" s="27">
+        <v>0</v>
+      </c>
+      <c r="G11" s="27">
+        <v>0</v>
+      </c>
+      <c r="H11" s="15">
+        <v>10</v>
+      </c>
+      <c r="I11" s="15">
+        <v>10</v>
+      </c>
+      <c r="J11" s="27">
+        <v>0</v>
+      </c>
+      <c r="K11" s="15">
+        <v>10</v>
+      </c>
+      <c r="L11" s="27">
+        <v>0</v>
+      </c>
+      <c r="M11" s="16"/>
+      <c r="N11" s="15">
+        <v>10</v>
+      </c>
+      <c r="O11" s="15">
+        <v>10</v>
+      </c>
+      <c r="P11" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="27">
+        <v>0</v>
+      </c>
+      <c r="R11" s="15">
+        <v>10</v>
+      </c>
+      <c r="S11" s="15">
+        <v>10</v>
+      </c>
+      <c r="T11" s="15">
+        <v>10</v>
+      </c>
+      <c r="U11" s="15">
+        <v>10</v>
+      </c>
+      <c r="V11" s="15">
+        <v>10</v>
+      </c>
+      <c r="W11" s="15">
+        <v>10</v>
+      </c>
+      <c r="X11" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="15">
+        <v>10</v>
+      </c>
+      <c r="Z11" s="15">
+        <v>10</v>
+      </c>
+      <c r="AA11" s="15">
+        <v>10</v>
+      </c>
+      <c r="AB11" s="15">
+        <v>10</v>
+      </c>
+      <c r="AC11" s="27">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="15">
+        <v>10</v>
+      </c>
+      <c r="AE11" s="15"/>
+      <c r="AF11" s="14">
+        <f t="shared" si="0"/>
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>6</v>
       </c>
@@ -2164,88 +2208,89 @@
       <c r="D12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="18">
-        <v>0</v>
-      </c>
-      <c r="F12" s="18">
-        <v>0</v>
-      </c>
-      <c r="G12" s="18">
-        <v>0</v>
-      </c>
-      <c r="H12" s="18">
-        <v>0</v>
-      </c>
-      <c r="I12" s="18">
-        <v>0</v>
-      </c>
-      <c r="J12" s="18">
-        <v>0</v>
-      </c>
-      <c r="K12" s="18">
-        <v>0</v>
-      </c>
-      <c r="L12" s="18">
-        <v>0</v>
-      </c>
-      <c r="M12" s="19"/>
-      <c r="N12" s="18">
-        <v>0</v>
-      </c>
-      <c r="O12" s="18">
-        <v>0</v>
-      </c>
-      <c r="P12" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="18">
-        <v>0</v>
-      </c>
-      <c r="R12" s="18">
-        <v>0</v>
-      </c>
-      <c r="S12" s="18">
-        <v>0</v>
-      </c>
-      <c r="T12" s="18">
-        <v>0</v>
-      </c>
-      <c r="U12" s="18">
-        <v>0</v>
-      </c>
-      <c r="V12" s="18">
-        <v>0</v>
-      </c>
-      <c r="W12" s="18">
-        <v>0</v>
-      </c>
-      <c r="X12" s="18">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="17">
-        <f>AVERAGE(E12:AD12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="E12" s="15">
+        <v>0</v>
+      </c>
+      <c r="F12" s="15">
+        <v>0</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0</v>
+      </c>
+      <c r="H12" s="15">
+        <v>0</v>
+      </c>
+      <c r="I12" s="15">
+        <v>0</v>
+      </c>
+      <c r="J12" s="15">
+        <v>0</v>
+      </c>
+      <c r="K12" s="15">
+        <v>0</v>
+      </c>
+      <c r="L12" s="15">
+        <v>0</v>
+      </c>
+      <c r="M12" s="16"/>
+      <c r="N12" s="15">
+        <v>0</v>
+      </c>
+      <c r="O12" s="15">
+        <v>0</v>
+      </c>
+      <c r="P12" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="15">
+        <v>0</v>
+      </c>
+      <c r="R12" s="15">
+        <v>0</v>
+      </c>
+      <c r="S12" s="15">
+        <v>0</v>
+      </c>
+      <c r="T12" s="15">
+        <v>0</v>
+      </c>
+      <c r="U12" s="15">
+        <v>0</v>
+      </c>
+      <c r="V12" s="15">
+        <v>0</v>
+      </c>
+      <c r="W12" s="15">
+        <v>0</v>
+      </c>
+      <c r="X12" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="15"/>
+      <c r="AF12" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>7</v>
       </c>
@@ -2255,88 +2300,89 @@
       <c r="D13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="18">
-        <v>0</v>
-      </c>
-      <c r="F13" s="18">
-        <v>0</v>
-      </c>
-      <c r="G13" s="18">
-        <v>0</v>
-      </c>
-      <c r="H13" s="18">
-        <v>0</v>
-      </c>
-      <c r="I13" s="18">
-        <v>0</v>
-      </c>
-      <c r="J13" s="18">
-        <v>0</v>
-      </c>
-      <c r="K13" s="18">
-        <v>0</v>
-      </c>
-      <c r="L13" s="18">
-        <v>0</v>
-      </c>
-      <c r="M13" s="19"/>
-      <c r="N13" s="18">
-        <v>0</v>
-      </c>
-      <c r="O13" s="18">
-        <v>0</v>
-      </c>
-      <c r="P13" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="18">
-        <v>0</v>
-      </c>
-      <c r="R13" s="18">
-        <v>0</v>
-      </c>
-      <c r="S13" s="18">
-        <v>0</v>
-      </c>
-      <c r="T13" s="18">
-        <v>0</v>
-      </c>
-      <c r="U13" s="18">
-        <v>0</v>
-      </c>
-      <c r="V13" s="18">
-        <v>0</v>
-      </c>
-      <c r="W13" s="18">
-        <v>0</v>
-      </c>
-      <c r="X13" s="18">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD13" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE13" s="17">
-        <f>AVERAGE(E13:AD13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="E13" s="41">
+        <v>0</v>
+      </c>
+      <c r="F13" s="41">
+        <v>0</v>
+      </c>
+      <c r="G13" s="41">
+        <v>0</v>
+      </c>
+      <c r="H13" s="41">
+        <v>0</v>
+      </c>
+      <c r="I13" s="41">
+        <v>0</v>
+      </c>
+      <c r="J13" s="41">
+        <v>0</v>
+      </c>
+      <c r="K13" s="41">
+        <v>0</v>
+      </c>
+      <c r="L13" s="41">
+        <v>0</v>
+      </c>
+      <c r="M13" s="16"/>
+      <c r="N13" s="41">
+        <v>0</v>
+      </c>
+      <c r="O13" s="41">
+        <v>0</v>
+      </c>
+      <c r="P13" s="41">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="41">
+        <v>0</v>
+      </c>
+      <c r="R13" s="41">
+        <v>0</v>
+      </c>
+      <c r="S13" s="41">
+        <v>0</v>
+      </c>
+      <c r="T13" s="41">
+        <v>0</v>
+      </c>
+      <c r="U13" s="41">
+        <v>0</v>
+      </c>
+      <c r="V13" s="41">
+        <v>0</v>
+      </c>
+      <c r="W13" s="41">
+        <v>0</v>
+      </c>
+      <c r="X13" s="41">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="41">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="41">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="41">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="41">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="41">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="41"/>
+      <c r="AF13" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>8</v>
       </c>
@@ -2346,88 +2392,89 @@
       <c r="D14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="18">
-        <v>0</v>
-      </c>
-      <c r="F14" s="18">
-        <v>0</v>
-      </c>
-      <c r="G14" s="18">
-        <v>0</v>
-      </c>
-      <c r="H14" s="18">
-        <v>0</v>
-      </c>
-      <c r="I14" s="18">
-        <v>0</v>
-      </c>
-      <c r="J14" s="18">
-        <v>0</v>
-      </c>
-      <c r="K14" s="18">
-        <v>0</v>
-      </c>
-      <c r="L14" s="18">
-        <v>0</v>
-      </c>
-      <c r="M14" s="19"/>
-      <c r="N14" s="18">
-        <v>0</v>
-      </c>
-      <c r="O14" s="18">
-        <v>0</v>
-      </c>
-      <c r="P14" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="18">
-        <v>0</v>
-      </c>
-      <c r="R14" s="18">
-        <v>0</v>
-      </c>
-      <c r="S14" s="18">
-        <v>0</v>
-      </c>
-      <c r="T14" s="18">
-        <v>0</v>
-      </c>
-      <c r="U14" s="18">
-        <v>0</v>
-      </c>
-      <c r="V14" s="18">
-        <v>0</v>
-      </c>
-      <c r="W14" s="18">
-        <v>0</v>
-      </c>
-      <c r="X14" s="18">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="17">
-        <f>AVERAGE(E14:AD14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="E14" s="15">
+        <v>10</v>
+      </c>
+      <c r="F14" s="15">
+        <v>10</v>
+      </c>
+      <c r="G14" s="15">
+        <v>10</v>
+      </c>
+      <c r="H14" s="27">
+        <v>0</v>
+      </c>
+      <c r="I14" s="27">
+        <v>0</v>
+      </c>
+      <c r="J14" s="27">
+        <v>0</v>
+      </c>
+      <c r="K14" s="15">
+        <v>10</v>
+      </c>
+      <c r="L14" s="15">
+        <v>10</v>
+      </c>
+      <c r="M14" s="16"/>
+      <c r="N14" s="27">
+        <v>0</v>
+      </c>
+      <c r="O14" s="15">
+        <v>10</v>
+      </c>
+      <c r="P14" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="15">
+        <v>10</v>
+      </c>
+      <c r="R14" s="15">
+        <v>10</v>
+      </c>
+      <c r="S14" s="15">
+        <v>10</v>
+      </c>
+      <c r="T14" s="27">
+        <v>0</v>
+      </c>
+      <c r="U14" s="15">
+        <v>10</v>
+      </c>
+      <c r="V14" s="15">
+        <v>10</v>
+      </c>
+      <c r="W14" s="15">
+        <v>10</v>
+      </c>
+      <c r="X14" s="15">
+        <v>10</v>
+      </c>
+      <c r="Y14" s="15">
+        <v>10</v>
+      </c>
+      <c r="Z14" s="15">
+        <v>10</v>
+      </c>
+      <c r="AA14" s="15">
+        <v>10</v>
+      </c>
+      <c r="AB14" s="15">
+        <v>10</v>
+      </c>
+      <c r="AC14" s="27">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="15">
+        <v>10</v>
+      </c>
+      <c r="AE14" s="15"/>
+      <c r="AF14" s="14">
+        <f t="shared" si="0"/>
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>9</v>
       </c>
@@ -2437,88 +2484,89 @@
       <c r="D15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="18">
-        <v>0</v>
-      </c>
-      <c r="F15" s="18">
-        <v>0</v>
-      </c>
-      <c r="G15" s="18">
-        <v>0</v>
-      </c>
-      <c r="H15" s="18">
-        <v>0</v>
-      </c>
-      <c r="I15" s="18">
-        <v>0</v>
-      </c>
-      <c r="J15" s="18">
-        <v>0</v>
-      </c>
-      <c r="K15" s="18">
-        <v>0</v>
-      </c>
-      <c r="L15" s="18">
-        <v>0</v>
-      </c>
-      <c r="M15" s="19"/>
-      <c r="N15" s="18">
-        <v>0</v>
-      </c>
-      <c r="O15" s="18">
-        <v>0</v>
-      </c>
-      <c r="P15" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="18">
-        <v>0</v>
-      </c>
-      <c r="R15" s="18">
-        <v>0</v>
-      </c>
-      <c r="S15" s="18">
-        <v>0</v>
-      </c>
-      <c r="T15" s="18">
-        <v>0</v>
-      </c>
-      <c r="U15" s="18">
-        <v>0</v>
-      </c>
-      <c r="V15" s="18">
-        <v>0</v>
-      </c>
-      <c r="W15" s="18">
-        <v>0</v>
-      </c>
-      <c r="X15" s="18">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="17">
-        <f>AVERAGE(E15:AD15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="E15" s="15">
+        <v>10</v>
+      </c>
+      <c r="F15" s="15">
+        <v>10</v>
+      </c>
+      <c r="G15" s="15">
+        <v>10</v>
+      </c>
+      <c r="H15" s="27">
+        <v>0</v>
+      </c>
+      <c r="I15" s="15">
+        <v>10</v>
+      </c>
+      <c r="J15" s="27">
+        <v>0</v>
+      </c>
+      <c r="K15" s="15">
+        <v>10</v>
+      </c>
+      <c r="L15" s="15">
+        <v>10</v>
+      </c>
+      <c r="M15" s="16"/>
+      <c r="N15" s="15">
+        <v>10</v>
+      </c>
+      <c r="O15" s="15">
+        <v>10</v>
+      </c>
+      <c r="P15" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q15" s="27">
+        <v>0</v>
+      </c>
+      <c r="R15" s="27">
+        <v>0</v>
+      </c>
+      <c r="S15" s="15">
+        <v>10</v>
+      </c>
+      <c r="T15" s="27">
+        <v>0</v>
+      </c>
+      <c r="U15" s="27">
+        <v>0</v>
+      </c>
+      <c r="V15" s="15">
+        <v>10</v>
+      </c>
+      <c r="W15" s="15">
+        <v>10</v>
+      </c>
+      <c r="X15" s="15">
+        <v>10</v>
+      </c>
+      <c r="Y15" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="15">
+        <v>10</v>
+      </c>
+      <c r="AA15" s="15">
+        <v>10</v>
+      </c>
+      <c r="AB15" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="27">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="15">
+        <v>10</v>
+      </c>
+      <c r="AE15" s="15"/>
+      <c r="AF15" s="14">
+        <f t="shared" si="0"/>
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <v>10</v>
       </c>
@@ -2528,89 +2576,98 @@
       <c r="D16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="18">
-        <v>0</v>
-      </c>
-      <c r="F16" s="18">
-        <v>0</v>
-      </c>
-      <c r="G16" s="18">
-        <v>0</v>
-      </c>
-      <c r="H16" s="18">
-        <v>0</v>
-      </c>
-      <c r="I16" s="18">
-        <v>0</v>
-      </c>
-      <c r="J16" s="18">
-        <v>0</v>
-      </c>
-      <c r="K16" s="18">
-        <v>0</v>
-      </c>
-      <c r="L16" s="18">
-        <v>0</v>
-      </c>
-      <c r="M16" s="19"/>
-      <c r="N16" s="18">
-        <v>0</v>
-      </c>
-      <c r="O16" s="18">
-        <v>0</v>
-      </c>
-      <c r="P16" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="18">
-        <v>0</v>
-      </c>
-      <c r="R16" s="18">
-        <v>0</v>
-      </c>
-      <c r="S16" s="18">
-        <v>0</v>
-      </c>
-      <c r="T16" s="18">
-        <v>0</v>
-      </c>
-      <c r="U16" s="18">
-        <v>0</v>
-      </c>
-      <c r="V16" s="18">
-        <v>0</v>
-      </c>
-      <c r="W16" s="18">
-        <v>0</v>
-      </c>
-      <c r="X16" s="18">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="18">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="18">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="18">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD16" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="17">
-        <f>AVERAGE(E16:AD16)</f>
+      <c r="E16" s="15">
+        <v>0</v>
+      </c>
+      <c r="F16" s="15">
+        <v>0</v>
+      </c>
+      <c r="G16" s="15">
+        <v>0</v>
+      </c>
+      <c r="H16" s="15">
+        <v>0</v>
+      </c>
+      <c r="I16" s="15">
+        <v>0</v>
+      </c>
+      <c r="J16" s="15">
+        <v>0</v>
+      </c>
+      <c r="K16" s="15">
+        <v>0</v>
+      </c>
+      <c r="L16" s="15">
+        <v>0</v>
+      </c>
+      <c r="M16" s="16"/>
+      <c r="N16" s="15">
+        <v>0</v>
+      </c>
+      <c r="O16" s="15">
+        <v>0</v>
+      </c>
+      <c r="P16" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="15">
+        <v>0</v>
+      </c>
+      <c r="R16" s="15">
+        <v>0</v>
+      </c>
+      <c r="S16" s="15">
+        <v>0</v>
+      </c>
+      <c r="T16" s="15">
+        <v>0</v>
+      </c>
+      <c r="U16" s="15">
+        <v>0</v>
+      </c>
+      <c r="V16" s="15">
+        <v>0</v>
+      </c>
+      <c r="W16" s="15">
+        <v>0</v>
+      </c>
+      <c r="X16" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="15"/>
+      <c r="AF16" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:AF2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="Y3:Z3"/>
     <mergeCell ref="O3:Q3"/>
@@ -2619,14 +2676,6 @@
     <mergeCell ref="R4:S4"/>
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="T4:U4"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:AE2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2641,7 +2690,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="4.28515625" customWidth="1"/>
@@ -2656,32 +2705,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>

</xml_diff>